<commit_message>
Alea 2: rest dimension with unity
</commit_message>
<xml_diff>
--- a/database/test.xlsx
+++ b/database/test.xlsx
@@ -8,27 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITU\S5\architecture-logiciel\foam\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B650D39-AEA7-4678-B144-2B31C34A4192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B41C3D9-E22D-4D1E-9457-896AC5E3666A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -55,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="65">
   <si>
     <t>Bloc</t>
   </si>
@@ -217,6 +205,39 @@
   </si>
   <si>
     <t>Forme usuelle la plus petite</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Longueur</t>
+  </si>
+  <si>
+    <t>Largeur</t>
+  </si>
+  <si>
+    <t>Hauteur</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Marge (30%)</t>
+  </si>
+  <si>
+    <t>Minimum acceptable</t>
+  </si>
+  <si>
+    <t>volume total</t>
+  </si>
+  <si>
+    <t>Somme volume</t>
+  </si>
+  <si>
+    <t>Validité</t>
+  </si>
+  <si>
+    <t>Transformation 2</t>
   </si>
 </sst>
 </file>
@@ -224,12 +245,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;???\ _€_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;??.0\ _€_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;???\ _€_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;??.0\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +269,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -381,27 +408,26 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -421,6 +447,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -701,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:V56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -818,7 +856,7 @@
       <c r="N3" s="2">
         <v>125000</v>
       </c>
-      <c r="O3" s="9">
+      <c r="O3" s="8">
         <f>K3*L3*M3</f>
         <v>0.96</v>
       </c>
@@ -868,7 +906,7 @@
       <c r="N4" s="2">
         <v>100000</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="8">
         <f t="shared" ref="O4:O6" si="3">K4*L4*M4</f>
         <v>0.7</v>
       </c>
@@ -918,7 +956,7 @@
       <c r="N5" s="2">
         <v>60000</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="8">
         <f t="shared" si="3"/>
         <v>0.34200000000000003</v>
       </c>
@@ -968,7 +1006,7 @@
       <c r="N6" s="2">
         <v>100</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6" s="8">
         <f t="shared" si="3"/>
         <v>1E-3</v>
       </c>
@@ -1004,11 +1042,11 @@
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="K12" s="19"/>
-      <c r="L12" s="20"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="19"/>
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="1" t="str">
@@ -1039,15 +1077,15 @@
         <f>N15</f>
         <v>B1</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="1" t="str">
@@ -1078,22 +1116,22 @@
         <f>N16</f>
         <v>B1</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="K14" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="L14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="M14" s="10" t="s">
+      <c r="M14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="N14" s="10" t="s">
+      <c r="N14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="O14" s="10" t="s">
+      <c r="O14" s="9" t="s">
         <v>22</v>
       </c>
       <c r="P14" s="1" t="s">
@@ -1133,7 +1171,7 @@
       <c r="L15" s="1">
         <v>50</v>
       </c>
-      <c r="M15" s="11">
+      <c r="M15" s="10">
         <f>K15*L15</f>
         <v>48</v>
       </c>
@@ -1148,23 +1186,23 @@
         <f>N3</f>
         <v>125000</v>
       </c>
-      <c r="R15" s="16">
+      <c r="R15" s="15">
         <f>E3</f>
         <v>38250000</v>
       </c>
-      <c r="S15" s="16">
+      <c r="S15" s="15">
         <f>P19</f>
         <v>31684307.409111802</v>
       </c>
-      <c r="T15" s="17" cm="1">
+      <c r="T15" s="16" cm="1">
         <f t="array" ref="T15">SUMPRODUCT(L15:L16,O15:O16)</f>
         <v>6030579.8435342899</v>
       </c>
-      <c r="U15" s="16">
+      <c r="U15" s="15">
         <f>S15+T15</f>
         <v>37714887.252646104</v>
       </c>
-      <c r="V15" s="16">
+      <c r="V15" s="15">
         <f>R15-U15</f>
         <v>535112.74735388195</v>
       </c>
@@ -1177,24 +1215,24 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K16" s="12">
         <f>O5</f>
         <v>0.34200000000000003</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="11">
         <v>60</v>
       </c>
-      <c r="M16" s="14">
+      <c r="M16" s="13">
         <f>K16*L16</f>
         <v>20.52</v>
       </c>
-      <c r="N16" s="12" t="s">
+      <c r="N16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="O16" s="13">
+      <c r="O16" s="12">
         <f>O5*$E$3/$G$3</f>
         <v>30100.092038656199</v>
       </c>
@@ -1211,57 +1249,57 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="J17" s="21" t="s">
+      <c r="J17" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="K18" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="L18" s="10" t="s">
+      <c r="L18" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="M18" s="10" t="s">
+      <c r="M18" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="N18" s="10" t="s">
+      <c r="N18" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="O18" s="10" t="s">
+      <c r="O18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P18" s="10" t="s">
+      <c r="P18" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="J19" s="12" t="s">
+      <c r="J19" s="11" t="s">
         <v>12</v>
       </c>
       <c r="K19" s="7">
         <f>G3</f>
         <v>434.6</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="11">
         <v>9</v>
       </c>
-      <c r="M19" s="12">
+      <c r="M19" s="11">
         <v>8</v>
       </c>
-      <c r="N19" s="12">
+      <c r="N19" s="11">
         <v>5</v>
       </c>
-      <c r="O19" s="12">
+      <c r="O19" s="11">
         <f>L19*M19*N19</f>
         <v>360</v>
       </c>
@@ -1274,15 +1312,15 @@
       <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="J20" s="22" t="s">
+      <c r="J20" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="24"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="23"/>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="1" t="s">
@@ -1369,15 +1407,15 @@
         <f>O19</f>
         <v>360</v>
       </c>
-      <c r="M22" s="11">
+      <c r="M22" s="10">
         <f>SUM(M15:M16)</f>
         <v>68.52</v>
       </c>
-      <c r="N22" s="11">
+      <c r="N22" s="10">
         <f>L22+M22</f>
         <v>428.52</v>
       </c>
-      <c r="O22" s="11">
+      <c r="O22" s="10">
         <f>G3-N22</f>
         <v>6.0799999999999299</v>
       </c>
@@ -1523,19 +1561,19 @@
         <f t="shared" ref="B33:G33" si="8">B13</f>
         <v>50</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="2">
         <f t="shared" si="8"/>
         <v>84491.4864242982</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="2">
         <f t="shared" si="8"/>
         <v>125000</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="2">
         <f t="shared" si="8"/>
         <v>4224574.3212149097</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="2">
         <f t="shared" si="8"/>
         <v>6250000</v>
       </c>
@@ -1553,19 +1591,19 @@
         <f t="shared" ref="B34:G34" si="9">B14</f>
         <v>60</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="2">
         <f t="shared" si="9"/>
         <v>30100.092038656199</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="2">
         <f t="shared" si="9"/>
         <v>60000</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="2">
         <f t="shared" si="9"/>
         <v>1806005.5223193699</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F34" s="2">
         <f t="shared" si="9"/>
         <v>3600000</v>
       </c>
@@ -1645,19 +1683,19 @@
         <f t="shared" ref="B41:G41" si="10">B13</f>
         <v>50</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="2">
         <f t="shared" si="10"/>
         <v>84491.4864242982</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D41" s="2">
         <f t="shared" si="10"/>
         <v>125000</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E41" s="2">
         <f t="shared" si="10"/>
         <v>4224574.3212149097</v>
       </c>
-      <c r="F41" s="8">
+      <c r="F41" s="2">
         <f t="shared" si="10"/>
         <v>6250000</v>
       </c>
@@ -1698,19 +1736,19 @@
         <f t="shared" ref="B42:G42" si="11">B14</f>
         <v>60</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42" s="2">
         <f t="shared" si="11"/>
         <v>30100.092038656199</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D42" s="2">
         <f t="shared" si="11"/>
         <v>60000</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E42" s="2">
         <f t="shared" si="11"/>
         <v>1806005.5223193699</v>
       </c>
-      <c r="F42" s="8">
+      <c r="F42" s="2">
         <f t="shared" si="11"/>
         <v>3600000</v>
       </c>
@@ -1724,27 +1762,27 @@
         <f>J5</f>
         <v>U3</v>
       </c>
-      <c r="L42" s="8">
+      <c r="L42" s="2">
         <f t="shared" ref="L42:Q42" si="12">K5</f>
         <v>1.9</v>
       </c>
-      <c r="M42" s="8">
+      <c r="M42" s="2">
         <f t="shared" si="12"/>
         <v>0.9</v>
       </c>
-      <c r="N42" s="8">
+      <c r="N42" s="2">
         <f t="shared" si="12"/>
         <v>0.2</v>
       </c>
-      <c r="O42" s="8">
+      <c r="O42" s="2">
         <f t="shared" si="12"/>
         <v>60000</v>
       </c>
-      <c r="P42" s="15">
+      <c r="P42" s="14">
         <f t="shared" si="12"/>
         <v>0.34200000000000003</v>
       </c>
-      <c r="Q42" s="8">
+      <c r="Q42" s="2">
         <f t="shared" si="12"/>
         <v>175438.596491228</v>
       </c>
@@ -1924,19 +1962,19 @@
         <f t="shared" ref="B52:G52" si="13">B13</f>
         <v>50</v>
       </c>
-      <c r="C52" s="8">
+      <c r="C52" s="2">
         <f t="shared" si="13"/>
         <v>84491.4864242982</v>
       </c>
-      <c r="D52" s="8">
+      <c r="D52" s="2">
         <f t="shared" si="13"/>
         <v>125000</v>
       </c>
-      <c r="E52" s="8">
+      <c r="E52" s="2">
         <f t="shared" si="13"/>
         <v>4224574.3212149097</v>
       </c>
-      <c r="F52" s="8">
+      <c r="F52" s="2">
         <f t="shared" si="13"/>
         <v>6250000</v>
       </c>
@@ -1977,19 +2015,19 @@
         <f t="shared" ref="B53:G53" si="14">B14</f>
         <v>60</v>
       </c>
-      <c r="C53" s="8">
+      <c r="C53" s="2">
         <f t="shared" si="14"/>
         <v>30100.092038656199</v>
       </c>
-      <c r="D53" s="8">
+      <c r="D53" s="2">
         <f t="shared" si="14"/>
         <v>60000</v>
       </c>
-      <c r="E53" s="8">
+      <c r="E53" s="2">
         <f t="shared" si="14"/>
         <v>1806005.5223193699</v>
       </c>
-      <c r="F53" s="8">
+      <c r="F53" s="2">
         <f t="shared" si="14"/>
         <v>3600000</v>
       </c>
@@ -2023,7 +2061,7 @@
         <f t="shared" si="15"/>
         <v>1E-3</v>
       </c>
-      <c r="Q53" s="8">
+      <c r="Q53" s="2">
         <f t="shared" si="15"/>
         <v>100000</v>
       </c>
@@ -2036,19 +2074,19 @@
       <c r="B54" s="1">
         <v>1</v>
       </c>
-      <c r="C54" s="8">
+      <c r="C54" s="2">
         <f>E22</f>
         <v>38250000</v>
       </c>
-      <c r="D54" s="8">
+      <c r="D54" s="2">
         <f>I54*$O$53</f>
         <v>43460000</v>
       </c>
-      <c r="E54" s="8">
+      <c r="E54" s="2">
         <f>C54*B54</f>
         <v>38250000</v>
       </c>
-      <c r="F54" s="8">
+      <c r="F54" s="2">
         <f>B54*D54</f>
         <v>43460000</v>
       </c>
@@ -2070,19 +2108,19 @@
       <c r="B55" s="1">
         <v>1</v>
       </c>
-      <c r="C55" s="8">
+      <c r="C55" s="2">
         <f>E23</f>
         <v>38250000</v>
       </c>
-      <c r="D55" s="8">
+      <c r="D55" s="2">
         <f>I55*$O$53</f>
         <v>43460000</v>
       </c>
-      <c r="E55" s="8">
+      <c r="E55" s="2">
         <f t="shared" ref="E55:E56" si="16">C55*B55</f>
         <v>38250000</v>
       </c>
-      <c r="F55" s="8">
+      <c r="F55" s="2">
         <f t="shared" ref="F55" si="17">B55*D55</f>
         <v>43460000</v>
       </c>
@@ -2104,19 +2142,19 @@
       <c r="B56" s="1">
         <v>1</v>
       </c>
-      <c r="C56" s="8">
+      <c r="C56" s="2">
         <f>E24</f>
         <v>31684307.409111802</v>
       </c>
-      <c r="D56" s="8">
+      <c r="D56" s="2">
         <f>I56*$O$53</f>
         <v>36000000</v>
       </c>
-      <c r="E56" s="8">
+      <c r="E56" s="2">
         <f t="shared" si="16"/>
         <v>31684307.409111802</v>
       </c>
-      <c r="F56" s="8">
+      <c r="F56" s="2">
         <f>B56*D56</f>
         <v>36000000</v>
       </c>
@@ -2142,4 +2180,593 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0B55FC-8A4A-468B-8C59-35825DF8FB97}">
+  <dimension ref="A1:S29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
+        <v>100</v>
+      </c>
+      <c r="C3" s="2">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2">
+        <f>B3*C3*D3</f>
+        <v>20000</v>
+      </c>
+      <c r="F3" s="2">
+        <f>E3*30%</f>
+        <v>6000</v>
+      </c>
+      <c r="G3" s="2">
+        <f>E3-F3</f>
+        <v>14000</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="2">
+        <v>16</v>
+      </c>
+      <c r="M3" s="2">
+        <v>4</v>
+      </c>
+      <c r="N3" s="2">
+        <v>2</v>
+      </c>
+      <c r="O3" s="2">
+        <v>20000</v>
+      </c>
+      <c r="P3" s="8">
+        <f>L3*M3*N3</f>
+        <v>128</v>
+      </c>
+      <c r="Q3" s="2">
+        <f>O3/(L3*M3*N3)</f>
+        <v>156.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <v>100</v>
+      </c>
+      <c r="C4" s="2">
+        <v>40</v>
+      </c>
+      <c r="D4" s="2">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2">
+        <f>B4*C4*D4</f>
+        <v>40000</v>
+      </c>
+      <c r="F4" s="2">
+        <f>E4*30%</f>
+        <v>12000</v>
+      </c>
+      <c r="G4" s="2">
+        <f>E4-F4</f>
+        <v>28000</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="2">
+        <v>10</v>
+      </c>
+      <c r="M4" s="2">
+        <v>7</v>
+      </c>
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2">
+        <v>12000</v>
+      </c>
+      <c r="P4" s="8">
+        <f>L4*M4*N4</f>
+        <v>70</v>
+      </c>
+      <c r="Q4" s="2">
+        <f t="shared" ref="Q4:Q6" si="0">O4/(L4*M4*N4)</f>
+        <v>171.42857142857142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="K5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="2">
+        <v>5</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="2">
+        <v>600</v>
+      </c>
+      <c r="P5" s="8">
+        <f>L5*M5*N5</f>
+        <v>5</v>
+      </c>
+      <c r="Q5" s="2">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="K6" s="1"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="K9" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="K10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="K11" s="1" t="str">
+        <f>$K$3</f>
+        <v>U1</v>
+      </c>
+      <c r="L11" s="4">
+        <f>P3</f>
+        <v>128</v>
+      </c>
+      <c r="M11" s="1">
+        <v>100</v>
+      </c>
+      <c r="N11" s="10">
+        <f>L11*M11</f>
+        <v>12800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="K12" s="1" t="str">
+        <f t="shared" ref="K12:K13" si="1">K4</f>
+        <v>U2</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" ref="L12:L13" si="2">P4</f>
+        <v>70</v>
+      </c>
+      <c r="M12" s="1">
+        <v>250</v>
+      </c>
+      <c r="N12" s="10">
+        <f t="shared" ref="N12:N13" si="3">L12*M12</f>
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="K13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>U3</v>
+      </c>
+      <c r="L13" s="4">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="M13" s="1">
+        <v>500</v>
+      </c>
+      <c r="N13" s="10">
+        <f>L13*M13</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="K14" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="27"/>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="K15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="K16" s="1">
+        <v>500</v>
+      </c>
+      <c r="L16" s="1">
+        <v>2</v>
+      </c>
+      <c r="M16" s="1">
+        <v>3</v>
+      </c>
+      <c r="N16" s="1">
+        <f>K16*L16*M16</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="17" spans="11:19">
+      <c r="K17" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+    </row>
+    <row r="18" spans="11:19">
+      <c r="K18" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" s="24"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="10">
+        <f>SUM(N11:N13)+N16</f>
+        <v>35800</v>
+      </c>
+    </row>
+    <row r="20" spans="11:19">
+      <c r="K20" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="P20" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+    </row>
+    <row r="21" spans="11:19">
+      <c r="K21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="11:19">
+      <c r="K22" s="1" t="str">
+        <f>K3</f>
+        <v>U1</v>
+      </c>
+      <c r="L22" s="4">
+        <f>P3</f>
+        <v>128</v>
+      </c>
+      <c r="M22" s="1">
+        <v>42</v>
+      </c>
+      <c r="N22" s="10">
+        <f>L22*M22</f>
+        <v>5376</v>
+      </c>
+      <c r="P22" s="1" t="str">
+        <f>K3</f>
+        <v>U1</v>
+      </c>
+      <c r="Q22" s="4">
+        <f>P3</f>
+        <v>128</v>
+      </c>
+      <c r="R22" s="1">
+        <v>42</v>
+      </c>
+      <c r="S22" s="10">
+        <f>Q22*R22</f>
+        <v>5376</v>
+      </c>
+    </row>
+    <row r="23" spans="11:19">
+      <c r="K23" s="1" t="str">
+        <f t="shared" ref="K23:K24" si="4">K4</f>
+        <v>U2</v>
+      </c>
+      <c r="L23" s="4">
+        <f t="shared" ref="L23:L24" si="5">P4</f>
+        <v>70</v>
+      </c>
+      <c r="M23" s="1">
+        <v>50</v>
+      </c>
+      <c r="N23" s="10">
+        <f t="shared" ref="N23:N24" si="6">L23*M23</f>
+        <v>3500</v>
+      </c>
+      <c r="P23" s="1" t="str">
+        <f t="shared" ref="P23:P24" si="7">K4</f>
+        <v>U2</v>
+      </c>
+      <c r="Q23" s="4">
+        <f t="shared" ref="Q23:Q24" si="8">P4</f>
+        <v>70</v>
+      </c>
+      <c r="R23" s="1">
+        <v>50</v>
+      </c>
+      <c r="S23" s="10">
+        <f t="shared" ref="S23:S24" si="9">Q23*R23</f>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="24" spans="11:19">
+      <c r="K24" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>U3</v>
+      </c>
+      <c r="L24" s="4">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="M24" s="1">
+        <v>1000</v>
+      </c>
+      <c r="N24" s="10">
+        <f t="shared" si="6"/>
+        <v>5000</v>
+      </c>
+      <c r="P24" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>U3</v>
+      </c>
+      <c r="Q24" s="4">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="R24" s="1">
+        <v>1000</v>
+      </c>
+      <c r="S24" s="10">
+        <f t="shared" si="9"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="25" spans="11:19">
+      <c r="K25" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="27"/>
+      <c r="P25" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="27"/>
+    </row>
+    <row r="26" spans="11:19">
+      <c r="K26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="11:19">
+      <c r="K27" s="1">
+        <v>50</v>
+      </c>
+      <c r="L27" s="1">
+        <v>2</v>
+      </c>
+      <c r="M27" s="1">
+        <v>1</v>
+      </c>
+      <c r="N27" s="1">
+        <f>K27*L27*M27</f>
+        <v>100</v>
+      </c>
+      <c r="P27" s="1">
+        <v>500</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>2</v>
+      </c>
+      <c r="R27" s="1">
+        <v>3</v>
+      </c>
+      <c r="S27" s="1">
+        <f>P27*Q27*R27</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="28" spans="11:19">
+      <c r="K28" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="P28" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q28" s="24"/>
+      <c r="R28" s="24"/>
+      <c r="S28" s="24"/>
+    </row>
+    <row r="29" spans="11:19">
+      <c r="K29" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="L29" s="24"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="10">
+        <f>SUM(N22:N24)+N27</f>
+        <v>13976</v>
+      </c>
+      <c r="P29" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q29" s="24"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="10">
+        <f>SUM(S22:S24)+S27</f>
+        <v>16876</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="P20:S20"/>
+    <mergeCell ref="P25:S25"/>
+    <mergeCell ref="P28:S28"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="K28:N28"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="K25:N25"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>